<commit_message>
ME-C2 work in progress
</commit_message>
<xml_diff>
--- a/WebsiteCreator/ImageCreators/ImageCreator.xlsx
+++ b/WebsiteCreator/ImageCreators/ImageCreator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Onedrive\Documents_Charl\Computer_Technical\Programming_GitHub\AustralianSchoolMaths\WebsiteCreator\ImageCreators\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AACA474-D872-46D8-8026-C5E00300697F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E83DC3B-C372-40F6-ADB2-5714DB11CCC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="3" xr2:uid="{95822D8F-9FFC-4F5D-9AE5-1C1FA9EB8246}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>X</t>
   </si>
@@ -108,9 +108,6 @@
   </si>
   <si>
     <t>Negative k</t>
-  </si>
-  <si>
-    <t>Rate of change directly proportional to the current quantity</t>
   </si>
   <si>
     <t>Proportionate to N, Positive k</t>
@@ -1384,12 +1381,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -1397,22 +1391,26 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-AU"/>
-              <a:t>Growth</a:t>
+              <a:rPr lang="en-AU" sz="1100">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Growth (positive</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-AU" baseline="0"/>
-              <a:t> (</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-AU"/>
-              <a:t>positive</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-AU" baseline="0"/>
+              <a:rPr lang="en-AU" sz="1100" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
               <a:t> value of k)</a:t>
             </a:r>
-            <a:endParaRPr lang="en-AU"/>
+            <a:endParaRPr lang="en-AU" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
           </a:p>
         </c:rich>
       </c:tx>
@@ -1420,8 +1418,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="1.3673447069116362E-2"/>
-          <c:y val="3.7036898672337483E-2"/>
+          <c:x val="1.6775231481481474E-2"/>
+          <c:y val="3.7037037037037035E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1437,12 +1435,9 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
+                <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -1460,8 +1455,8 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.18730555555555559"/>
-          <c:y val="0.17634259259259263"/>
+          <c:x val="0.19008333333333335"/>
+          <c:y val="0.17634260589689063"/>
           <c:w val="0.77502777777777776"/>
           <c:h val="0.63670567220764074"/>
         </c:manualLayout>
@@ -1591,93 +1586,93 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>ME_C1_Graphs!$C$10:$C$37</c:f>
+              <c:f>ME_C1_Graphs!$E$10:$E$37</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.0_);\(#,##0.0\);\-??</c:formatCode>
                 <c:ptCount val="28"/>
                 <c:pt idx="0">
-                  <c:v>800</c:v>
+                  <c:v>830</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>884.13673446051814</c:v>
+                  <c:v>914.13673446051814</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>977.12220652813585</c:v>
+                  <c:v>1007.1222065281358</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1079.8870460608025</c:v>
+                  <c:v>1109.8870460608025</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1193.4597581130163</c:v>
+                  <c:v>1223.4597581130163</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1318.9770165601026</c:v>
+                  <c:v>1348.9770165601026</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1457.6950403124074</c:v>
+                  <c:v>1487.6950403124074</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1611.0021659763813</c:v>
+                  <c:v>1641.0021659763813</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1780.4327427939743</c:v>
+                  <c:v>1810.4327427939743</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1967.6824889255599</c:v>
+                  <c:v>1997.6824889255599</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2174.6254627672361</c:v>
+                  <c:v>2204.6254627672361</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2403.3328191571468</c:v>
+                  <c:v>2433.3328191571468</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2656.0935381892386</c:v>
+                  <c:v>2686.0935381892386</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2935.4373340953957</c:v>
+                  <c:v>2965.4373340953957</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3244.1599734757401</c:v>
+                  <c:v>3274.1599734757401</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3585.3512562704518</c:v>
+                  <c:v>3615.3512562704518</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3962.4259395160921</c:v>
+                  <c:v>3992.4259395160921</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4379.1579133817604</c:v>
+                  <c:v>4409.1579133817604</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>4839.7179715303573</c:v>
+                  <c:v>4869.7179715303573</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>5348.7155538234165</c:v>
+                  <c:v>5378.7155538234165</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>5911.2448791445204</c:v>
+                  <c:v>5941.2448791445204</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>6532.9359300541209</c:v>
+                  <c:v>6562.9359300541209</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>7220.0107995472972</c:v>
+                  <c:v>7250.0107995472972</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>7979.3459638517788</c:v>
+                  <c:v>8009.3459638517788</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>8818.5411045132842</c:v>
+                  <c:v>8848.5411045132842</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>9745.9951685627784</c:v>
+                  <c:v>9775.9951685627784</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>10770.990428001352</c:v>
+                  <c:v>10800.990428001352</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>11903.785379898269</c:v>
+                  <c:v>11933.785379898269</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2022,1238 +2017,6 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-AU"/>
-              <a:t>Decay (negative</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-AU" baseline="0"/>
-              <a:t> value of k)</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-AU"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="1.922900262467192E-2"/>
-          <c:y val="3.3387263635841137E-2"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="smoothMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>ME_C1_Graphs!$C$9</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Proportionate to N, Positive k</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-              <a:tailEnd type="triangle"/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>ME_C1_Graphs!$B$10:$B$37</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="28"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>23</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>27</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>ME_C1_Graphs!$D$10:$D$37</c:f>
-              <c:numCache>
-                <c:formatCode>#,##0.0_);\(#,##0.0\);\-??</c:formatCode>
-                <c:ptCount val="28"/>
-                <c:pt idx="0">
-                  <c:v>800</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>723.86993442876758</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>654.98460246238551</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>592.65457654537431</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>536.25603682851147</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>485.22452777010676</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>439.04930887522113</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>397.26824303312759</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>359.46317129377724</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>325.25572779247926</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>294.30355293715388</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>266.29686695846362</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>240.95536952976161</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>218.02543442721009</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>197.27757115328515</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>178.50412811874386</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>161.5172143957243</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>146.14681924218769</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>132.23911057726923</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>119.65489537810802</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>108.26822658929017</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>97.965142602385527</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>88.642526689867097</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>80.207074978242971</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>72.574362631529979</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>65.667998899119041</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>59.418862571467102</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>53.764410191799804</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-5F8F-42CB-92F3-9E934E3A4943}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="2124773040"/>
-        <c:axId val="2124760080"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="2124773040"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:min val="-10"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-AU"/>
-                  <a:t>time (t)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-            <a:headEnd type="arrow"/>
-            <a:tailEnd type="arrow"/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="t" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="2124760080"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="2124760080"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:max val="900"/>
-          <c:min val="-200"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-AU"/>
-                  <a:t>Quantity</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-AU" baseline="0"/>
-                  <a:t> (N)</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-AU"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout>
-            <c:manualLayout>
-              <c:xMode val="edge"/>
-              <c:yMode val="edge"/>
-              <c:x val="0.18611111111111112"/>
-              <c:y val="0.54555519101778949"/>
-            </c:manualLayout>
-          </c:layout>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="#,##0.0_);\(#,##0.0\);\-??" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="none"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-            <a:headEnd type="arrow"/>
-            <a:tailEnd type="arrow"/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="2124773040"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-        <c:majorUnit val="800"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:noFill/>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:noFill/>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-AU" sz="1100">
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000"/>
-                </a:solidFill>
-              </a:rPr>
-              <a:t>Growth (positive</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-AU" sz="1100" baseline="0">
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000"/>
-                </a:solidFill>
-              </a:rPr>
-              <a:t> value of k)</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-AU" sz="1100">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:endParaRPr>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="1.6775231481481474E-2"/>
-          <c:y val="3.7037037037037035E-2"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.19008333333333335"/>
-          <c:y val="0.17634260589689063"/>
-          <c:w val="0.77502777777777776"/>
-          <c:h val="0.63670567220764074"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:scatterChart>
-        <c:scatterStyle val="smoothMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>ME_C1_Graphs!$C$9</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Proportionate to N, Positive k</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-              <a:tailEnd type="triangle"/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>ME_C1_Graphs!$B$10:$B$37</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="28"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>23</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>27</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>ME_C1_Graphs!$E$10:$E$37</c:f>
-              <c:numCache>
-                <c:formatCode>#,##0.0_);\(#,##0.0\);\-??</c:formatCode>
-                <c:ptCount val="28"/>
-                <c:pt idx="0">
-                  <c:v>830</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>914.13673446051814</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1007.1222065281358</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1109.8870460608025</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1223.4597581130163</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1348.9770165601026</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1487.6950403124074</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1641.0021659763813</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1810.4327427939743</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1997.6824889255599</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2204.6254627672361</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2433.3328191571468</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>2686.0935381892386</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>2965.4373340953957</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>3274.1599734757401</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>3615.3512562704518</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>3992.4259395160921</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>4409.1579133817604</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>4869.7179715303573</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>5378.7155538234165</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>5941.2448791445204</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>6562.9359300541209</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>7250.0107995472972</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>8009.3459638517788</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>8848.5411045132842</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>9775.9951685627784</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>10800.990428001352</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>11933.785379898269</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-9F60-4285-B470-D879BCBCDE94}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="2124773040"/>
-        <c:axId val="2124760080"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="2124773040"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:min val="-10"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-AU"/>
-                  <a:t>time (t)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-            <a:headEnd type="arrow"/>
-            <a:tailEnd type="arrow"/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="t" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="2124760080"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="2124760080"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:min val="-5000"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-AU"/>
-                  <a:t>Quantity</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-AU" baseline="0"/>
-                  <a:t> (N)</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-AU"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout>
-            <c:manualLayout>
-              <c:xMode val="edge"/>
-              <c:yMode val="edge"/>
-              <c:x val="0.20555555555555552"/>
-              <c:y val="0.26042432195975501"/>
-            </c:manualLayout>
-          </c:layout>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="#,##0.0_);\(#,##0.0\);\-??" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="none"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-            <a:headEnd type="arrow"/>
-            <a:tailEnd type="arrow"/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="2124773040"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:noFill/>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:noFill/>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
               <a:rPr lang="en-AU" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000"/>
@@ -5801,86 +4564,6 @@
 </file>
 
 <file path=xl/charts/colors14.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors15.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors16.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -8821,1038 +7504,6 @@
 </file>
 
 <file path=xl/charts/style14.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style15.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style16.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -17641,660 +15292,6 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>301625</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>3175</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>354425</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>112625</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD7BEA9A-BCDC-4AB3-3E12-BD4E4CA1207C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>69850</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>395700</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>179300</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1AE0E22E-E512-43EE-B9BA-F86806A9DCC2}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>412750</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>165100</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>450850</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="TextBox 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B4B00F7-33B7-9CA1-65D9-62E83C9878F3}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="15938500" y="1498600"/>
-          <a:ext cx="971550" cy="457200"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-AU" sz="1100"/>
-            <a:t>Initial quanity</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-AU" sz="1100" baseline="0"/>
-            <a:t> = A</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-AU" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>273050</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>82550</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>603250</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="TextBox 5">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ADE5B891-D8F6-E8EE-5E60-A95FE386A54C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9702800" y="2324100"/>
-          <a:ext cx="939800" cy="438150"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-AU" sz="1100"/>
-            <a:t>Initial quanity</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-AU" sz="1100" baseline="0"/>
-            <a:t> = A</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-AU" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>549275</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="768800" cy="180690"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="7" name="TextBox 6">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4DCD0A7C-3E46-79C2-E580-D30E89DE6120}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="12417425" y="2346325"/>
-              <a:ext cx="768800" cy="180690"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr/>
-              <a14:m>
-                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
-                  <m:oMathParaPr>
-                    <m:jc m:val="centerGroup"/>
-                  </m:oMathParaPr>
-                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
-                    <m:r>
-                      <a:rPr lang="en-AU" sz="1100" i="1">
-                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      </a:rPr>
-                      <m:t>𝑁</m:t>
-                    </m:r>
-                    <m:d>
-                      <m:dPr>
-                        <m:ctrlPr>
-                          <a:rPr lang="en-AU" sz="1100" i="1">
-                            <a:solidFill>
-                              <a:srgbClr val="836967"/>
-                            </a:solidFill>
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                        </m:ctrlPr>
-                      </m:dPr>
-                      <m:e>
-                        <m:r>
-                          <a:rPr lang="en-AU" sz="1100" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>𝑡</m:t>
-                        </m:r>
-                      </m:e>
-                    </m:d>
-                    <m:r>
-                      <a:rPr lang="en-AU" sz="1100" i="0">
-                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      </a:rPr>
-                      <m:t>=</m:t>
-                    </m:r>
-                    <m:r>
-                      <a:rPr lang="en-AU" sz="1100" i="1">
-                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      </a:rPr>
-                      <m:t>𝐴</m:t>
-                    </m:r>
-                    <m:sSup>
-                      <m:sSupPr>
-                        <m:ctrlPr>
-                          <a:rPr lang="en-AU" sz="1100" i="1">
-                            <a:solidFill>
-                              <a:srgbClr val="836967"/>
-                            </a:solidFill>
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                        </m:ctrlPr>
-                      </m:sSupPr>
-                      <m:e>
-                        <m:r>
-                          <a:rPr lang="en-AU" sz="1100" i="0">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>ⅇ</m:t>
-                        </m:r>
-                      </m:e>
-                      <m:sup>
-                        <m:r>
-                          <a:rPr lang="en-AU" sz="1100" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>𝑘𝑡</m:t>
-                        </m:r>
-                      </m:sup>
-                    </m:sSup>
-                  </m:oMath>
-                </m:oMathPara>
-              </a14:m>
-              <a:endParaRPr lang="en-AU" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Choice>
-      <mc:Fallback xmlns="">
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="7" name="TextBox 6">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4DCD0A7C-3E46-79C2-E580-D30E89DE6120}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="12417425" y="2346325"/>
-              <a:ext cx="768800" cy="180690"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr/>
-              <a:r>
-                <a:rPr lang="en-AU" sz="1100" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>𝑁</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-AU" sz="1100" i="0">
-                  <a:solidFill>
-                    <a:srgbClr val="836967"/>
-                  </a:solidFill>
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>(</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-AU" sz="1100" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>𝑡)=𝐴ⅇ</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-AU" sz="1100" i="0">
-                  <a:solidFill>
-                    <a:srgbClr val="836967"/>
-                  </a:solidFill>
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>^</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-AU" sz="1100" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>𝑘𝑡</a:t>
-              </a:r>
-              <a:endParaRPr lang="en-AU" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>339725</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="768800" cy="180690"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="8" name="TextBox 7">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13F0E291-DE63-A2DE-14C4-4A149899BDBB}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="18303875" y="2771775"/>
-              <a:ext cx="768800" cy="180690"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr/>
-              <a14:m>
-                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
-                  <m:oMathParaPr>
-                    <m:jc m:val="centerGroup"/>
-                  </m:oMathParaPr>
-                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
-                    <m:r>
-                      <a:rPr lang="en-AU" sz="1100" i="1">
-                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      </a:rPr>
-                      <m:t>𝑁</m:t>
-                    </m:r>
-                    <m:d>
-                      <m:dPr>
-                        <m:ctrlPr>
-                          <a:rPr lang="en-AU" sz="1100" i="1">
-                            <a:solidFill>
-                              <a:srgbClr val="836967"/>
-                            </a:solidFill>
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                        </m:ctrlPr>
-                      </m:dPr>
-                      <m:e>
-                        <m:r>
-                          <a:rPr lang="en-AU" sz="1100" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>𝑡</m:t>
-                        </m:r>
-                      </m:e>
-                    </m:d>
-                    <m:r>
-                      <a:rPr lang="en-AU" sz="1100" i="0">
-                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      </a:rPr>
-                      <m:t>=</m:t>
-                    </m:r>
-                    <m:r>
-                      <a:rPr lang="en-AU" sz="1100" i="1">
-                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      </a:rPr>
-                      <m:t>𝐴</m:t>
-                    </m:r>
-                    <m:sSup>
-                      <m:sSupPr>
-                        <m:ctrlPr>
-                          <a:rPr lang="en-AU" sz="1100" i="1">
-                            <a:solidFill>
-                              <a:srgbClr val="836967"/>
-                            </a:solidFill>
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                        </m:ctrlPr>
-                      </m:sSupPr>
-                      <m:e>
-                        <m:r>
-                          <a:rPr lang="en-AU" sz="1100" i="0">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>ⅇ</m:t>
-                        </m:r>
-                      </m:e>
-                      <m:sup>
-                        <m:r>
-                          <a:rPr lang="en-AU" sz="1100" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>𝑘𝑡</m:t>
-                        </m:r>
-                      </m:sup>
-                    </m:sSup>
-                  </m:oMath>
-                </m:oMathPara>
-              </a14:m>
-              <a:endParaRPr lang="en-AU" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Choice>
-      <mc:Fallback xmlns="">
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="8" name="TextBox 7">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13F0E291-DE63-A2DE-14C4-4A149899BDBB}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="18303875" y="2771775"/>
-              <a:ext cx="768800" cy="180690"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr/>
-              <a:r>
-                <a:rPr lang="en-AU" sz="1100" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>𝑁</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-AU" sz="1100" i="0">
-                  <a:solidFill>
-                    <a:srgbClr val="836967"/>
-                  </a:solidFill>
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>(</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-AU" sz="1100" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>𝑡)=𝐴ⅇ</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-AU" sz="1100" i="0">
-                  <a:solidFill>
-                    <a:srgbClr val="836967"/>
-                  </a:solidFill>
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>^</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-AU" sz="1100" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>𝑘𝑡</a:t>
-              </a:r>
-              <a:endParaRPr lang="en-AU" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>10</xdr:col>
       <xdr:colOff>434975</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>174625</xdr:rowOff>
@@ -18322,7 +15319,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -18431,7 +15428,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -20031,7 +17028,7 @@
   <dimension ref="B2:Q37"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="P47" sqref="P46:P47"/>
+      <selection activeCell="Y12" sqref="Y12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -20044,9 +17041,7 @@
   <sheetData>
     <row r="2" spans="2:11" ht="17" x14ac:dyDescent="0.4">
       <c r="B2" s="12"/>
-      <c r="K2" s="14" t="s">
-        <v>23</v>
-      </c>
+      <c r="K2" s="14"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
@@ -20074,7 +17069,7 @@
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C7">
         <v>30</v>
@@ -20085,16 +17080,16 @@
         <v>19</v>
       </c>
       <c r="C9" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="E9" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="10" t="s">
-        <v>26</v>
-      </c>
       <c r="F9" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.35">
@@ -20370,7 +17365,7 @@
         <v>2686.0935381892386</v>
       </c>
       <c r="K22" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="2:17" x14ac:dyDescent="0.35">

</xml_diff>